<commit_message>
Refactor ExportController and SocioController
- Remove unnecessary page margin settings in ExportController
- Add validation to check if DNI already exists in SocioController store method
- Update SocioController store method to handle date format
- Add file validation and storage logic in PolizaController store and update methods
</commit_message>
<xml_diff>
--- a/storage/app/public/plantillas/SUBPRODUCTO K5 - copia.xlsx
+++ b/storage/app/public/plantillas/SUBPRODUCTO K5 - copia.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIGUEL\Desktop\Kyrema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIGUEL\Desktop\backend-kyrema\storage\app\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8EBE86-7C0D-458D-96B1-3897FA26F961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6C9649-4637-40B8-83E9-0E16F7419A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,19 +25,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="1">
-  <si>
-    <t>K5</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>adad</t>
+  </si>
+  <si>
+    <t>sadsad</t>
+  </si>
+  <si>
+    <t>dasdsa</t>
+  </si>
+  <si>
+    <t>dsad</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>dad</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>das</t>
+  </si>
+  <si>
+    <t>dadsa</t>
+  </si>
+  <si>
+    <t>dasda</t>
+  </si>
+  <si>
+    <t>dadas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -63,8 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,39 +397,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="G3:H5"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G3" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G4" t="s">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+    </row>
+    <row r="49" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+    </row>
+    <row r="50" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+    </row>
+    <row r="51" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+    </row>
+    <row r="52" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+    </row>
+    <row r="55" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="K55" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <picture r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>